<commit_message>
Change : Updated for fieldvalues
</commit_message>
<xml_diff>
--- a/MRK.HIV.Digitized.by.DRE.-5.10.18.-.2.xlsx
+++ b/MRK.HIV.Digitized.by.DRE.-5.10.18.-.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="0" windowWidth="15705" windowHeight="12810" activeTab="1"/>
+    <workbookView xWindow="255" yWindow="0" windowWidth="15705" windowHeight="12810"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
@@ -3998,9 +3998,9 @@
   </sheetPr>
   <dimension ref="A1:AL112"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD91" sqref="AD91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10779,11 +10779,11 @@
   </sheetPr>
   <dimension ref="A1:CB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="BG8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="BU8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="BJ21" sqref="BJ21"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10791,7 +10791,7 @@
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="4" width="84.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="20" width="14.42578125" customWidth="1"/>
     <col min="21" max="21" width="58.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17.140625" style="120" customWidth="1"/>
@@ -19736,10 +19736,10 @@
   <dimension ref="A1:CU328"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="CI274" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="7" topLeftCell="CM8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="CT279" activeCellId="1" sqref="CU276 CT279"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -19747,9 +19747,9 @@
     <col min="1" max="1" width="11.85546875" style="88" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="88" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" style="87" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="106" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="106" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="87" customWidth="1"/>
+    <col min="6" max="6" width="117.85546875" style="87" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="14.42578125" style="88" customWidth="1"/>
     <col min="10" max="10" width="18.7109375" style="88" bestFit="1" customWidth="1"/>
     <col min="11" max="64" width="14.42578125" style="88" customWidth="1"/>

</xml_diff>

<commit_message>
Change : Updated excel
</commit_message>
<xml_diff>
--- a/MRK.HIV.Digitized.by.DRE.-5.10.18.-.2.xlsx
+++ b/MRK.HIV.Digitized.by.DRE.-5.10.18.-.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="0" windowWidth="15705" windowHeight="12810" activeTab="1"/>
+    <workbookView xWindow="255" yWindow="0" windowWidth="15705" windowHeight="12810"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
@@ -3998,9 +3998,9 @@
   </sheetPr>
   <dimension ref="A1:AL112"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD91" sqref="AD91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10779,11 +10779,11 @@
   </sheetPr>
   <dimension ref="A1:CB75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="BG8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="BU8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="BJ21" sqref="BJ21"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -10791,7 +10791,7 @@
     <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="4" width="84.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="20" width="14.42578125" customWidth="1"/>
     <col min="21" max="21" width="58.28515625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17.140625" style="120" customWidth="1"/>
@@ -19736,10 +19736,10 @@
   <dimension ref="A1:CU328"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="CI274" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="7" topLeftCell="CM8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="CT279" activeCellId="1" sqref="CU276 CT279"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -19747,9 +19747,9 @@
     <col min="1" max="1" width="11.85546875" style="88" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" style="88" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" style="87" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="106" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" style="106" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="88" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="87" customWidth="1"/>
+    <col min="6" max="6" width="117.85546875" style="87" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="14.42578125" style="88" customWidth="1"/>
     <col min="10" max="10" width="18.7109375" style="88" bestFit="1" customWidth="1"/>
     <col min="11" max="64" width="14.42578125" style="88" customWidth="1"/>

</xml_diff>